<commit_message>
Adjusted symmetry metric, finished
</commit_message>
<xml_diff>
--- a/test_short/heatmaps/symmetry_results.xlsx
+++ b/test_short/heatmaps/symmetry_results.xlsx
@@ -498,34 +498,34 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>0.06192129629629629</v>
+        <v>1.123842592592593</v>
       </c>
       <c r="D2" t="n">
-        <v>0.07696759259259259</v>
+        <v>1.153935185185185</v>
       </c>
       <c r="E2" t="n">
-        <v>0.470775462962963</v>
+        <v>1.941550925925926</v>
       </c>
       <c r="F2" t="n">
-        <v>0.06192129629629629</v>
+        <v>1.123842592592593</v>
       </c>
       <c r="G2" t="n">
-        <v>0.04021990740740741</v>
+        <v>1.080439814814815</v>
       </c>
       <c r="H2" t="n">
-        <v>0.06481481481481481</v>
+        <v>1.12962962962963</v>
       </c>
       <c r="I2" t="n">
-        <v>0.06481481481481481</v>
+        <v>1.12962962962963</v>
       </c>
       <c r="J2" t="n">
-        <v>0.06481481481481481</v>
+        <v>1.12962962962963</v>
       </c>
       <c r="K2" t="n">
-        <v>0.04021990740740741</v>
+        <v>1.080439814814815</v>
       </c>
       <c r="L2" t="n">
-        <v>0.06192129629629629</v>
+        <v>1.123842592592593</v>
       </c>
     </row>
     <row r="3">
@@ -542,28 +542,28 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>0.008264462809917356</v>
+        <v>1.016528925619835</v>
       </c>
       <c r="H3" t="n">
-        <v>0.008264462809917356</v>
+        <v>1.016528925619835</v>
       </c>
       <c r="I3" t="n">
-        <v>0.008264462809917356</v>
+        <v>1.016528925619835</v>
       </c>
       <c r="J3" t="n">
-        <v>0.008264462809917356</v>
+        <v>1.016528925619835</v>
       </c>
       <c r="K3" t="n">
-        <v>0.008264462809917356</v>
+        <v>1.016528925619835</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -573,35 +573,35 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1405529953917051</v>
+        <v>1.28110599078341</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1405529953917051</v>
+        <v>1.28110599078341</v>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>0.228110599078341</v>
+        <v>1.456221198156682</v>
       </c>
       <c r="F4" t="n">
-        <v>0.141705069124424</v>
+        <v>1.283410138248848</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1705069124423963</v>
+        <v>1.341013824884793</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1705069124423963</v>
+        <v>1.341013824884793</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1705069124423963</v>
+        <v>1.341013824884793</v>
       </c>
       <c r="K4" t="n">
         <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>0.141705069124424</v>
+        <v>1.283410138248848</v>
       </c>
     </row>
     <row r="5">
@@ -649,35 +649,35 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.02209944751381215</v>
+        <v>1.044198895027624</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4990791896869245</v>
+        <v>1.998158379373849</v>
       </c>
       <c r="D6" t="n">
-        <v>0.02209944751381215</v>
+        <v>1.044198895027624</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4990791896869245</v>
+        <v>1.998158379373849</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
-        <v>0.1298342541436464</v>
+        <v>1.259668508287293</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1298342541436464</v>
+        <v>1.259668508287293</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1298342541436464</v>
+        <v>1.259668508287293</v>
       </c>
       <c r="J6" t="n">
-        <v>0.1298342541436464</v>
+        <v>1.259668508287293</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1298342541436464</v>
+        <v>1.259668508287293</v>
       </c>
       <c r="L6" t="n">
-        <v>0.4990791896869245</v>
+        <v>1.998158379373849</v>
       </c>
     </row>
     <row r="7">
@@ -687,35 +687,35 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.485471296952516</v>
+        <v>1.970942593905032</v>
       </c>
       <c r="C7" t="n">
-        <v>0.485471296952516</v>
+        <v>1.970942593905032</v>
       </c>
       <c r="D7" t="n">
-        <v>0.485471296952516</v>
+        <v>1.970942593905032</v>
       </c>
       <c r="E7" t="n">
-        <v>0.485471296952516</v>
+        <v>1.970942593905032</v>
       </c>
       <c r="F7" t="n">
-        <v>0.485471296952516</v>
+        <v>1.970942593905032</v>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>0.485471296952516</v>
+        <v>1.970942593905032</v>
       </c>
       <c r="I7" t="n">
-        <v>0.485471296952516</v>
+        <v>1.970942593905032</v>
       </c>
       <c r="J7" t="n">
-        <v>0.485471296952516</v>
+        <v>1.970942593905032</v>
       </c>
       <c r="K7" t="n">
-        <v>0.485471296952516</v>
+        <v>1.970942593905032</v>
       </c>
       <c r="L7" t="n">
-        <v>0.485471296952516</v>
+        <v>1.970942593905032</v>
       </c>
     </row>
     <row r="8">
@@ -725,35 +725,35 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4936014625228519</v>
+        <v>1.987202925045704</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4936014625228519</v>
+        <v>1.987202925045704</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4936014625228519</v>
+        <v>1.987202925045704</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4936014625228519</v>
+        <v>1.987202925045704</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4936014625228519</v>
+        <v>1.987202925045704</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4936014625228519</v>
+        <v>1.987202925045704</v>
       </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>0.4936014625228519</v>
+        <v>1.987202925045704</v>
       </c>
       <c r="J8" t="n">
-        <v>0.4936014625228519</v>
+        <v>1.987202925045704</v>
       </c>
       <c r="K8" t="n">
-        <v>0.4936014625228519</v>
+        <v>1.987202925045704</v>
       </c>
       <c r="L8" t="n">
-        <v>0.4936014625228519</v>
+        <v>1.987202925045704</v>
       </c>
     </row>
     <row r="9">
@@ -763,35 +763,35 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.4987714987714988</v>
+        <v>1.997542997542998</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4987714987714988</v>
+        <v>1.997542997542998</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4987714987714988</v>
+        <v>1.997542997542998</v>
       </c>
       <c r="E9" t="n">
-        <v>0.4987714987714988</v>
+        <v>1.997542997542998</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4987714987714988</v>
+        <v>1.997542997542998</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4987714987714988</v>
+        <v>1.997542997542998</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4987714987714988</v>
+        <v>1.997542997542998</v>
       </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
-        <v>0.4987714987714988</v>
+        <v>1.997542997542998</v>
       </c>
       <c r="K9" t="n">
-        <v>0.4987714987714988</v>
+        <v>1.997542997542998</v>
       </c>
       <c r="L9" t="n">
-        <v>0.4987714987714988</v>
+        <v>1.997542997542998</v>
       </c>
     </row>
     <row r="10">
@@ -801,35 +801,35 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4983818770226537</v>
+        <v>1.996763754045308</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4983818770226537</v>
+        <v>1.996763754045308</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4983818770226537</v>
+        <v>1.996763754045308</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4983818770226537</v>
+        <v>1.996763754045308</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4983818770226537</v>
+        <v>1.996763754045308</v>
       </c>
       <c r="G10" t="n">
-        <v>0.4983818770226537</v>
+        <v>1.996763754045308</v>
       </c>
       <c r="H10" t="n">
-        <v>0.4983818770226537</v>
+        <v>1.996763754045308</v>
       </c>
       <c r="I10" t="n">
-        <v>0.4983818770226537</v>
+        <v>1.996763754045308</v>
       </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
-        <v>0.4983818770226537</v>
+        <v>1.996763754045308</v>
       </c>
       <c r="L10" t="n">
-        <v>0.4983818770226537</v>
+        <v>1.996763754045308</v>
       </c>
     </row>
     <row r="11">
@@ -839,35 +839,35 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.4931350114416476</v>
+        <v>1.986270022883295</v>
       </c>
       <c r="C11" t="n">
-        <v>0.4931350114416476</v>
+        <v>1.986270022883295</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4931350114416476</v>
+        <v>1.986270022883295</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4931350114416476</v>
+        <v>1.986270022883295</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4931350114416476</v>
+        <v>1.986270022883295</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4931350114416476</v>
+        <v>1.986270022883295</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4931350114416476</v>
+        <v>1.986270022883295</v>
       </c>
       <c r="I11" t="n">
-        <v>0.4931350114416476</v>
+        <v>1.986270022883295</v>
       </c>
       <c r="J11" t="n">
-        <v>0.4931350114416476</v>
+        <v>1.986270022883295</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="n">
-        <v>0.4931350114416476</v>
+        <v>1.986270022883295</v>
       </c>
     </row>
     <row r="12">
@@ -880,31 +880,31 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>0.05178907721280603</v>
+        <v>1.103578154425612</v>
       </c>
       <c r="H12" t="n">
-        <v>0.05178907721280603</v>
+        <v>1.103578154425612</v>
       </c>
       <c r="I12" t="n">
-        <v>0.05178907721280603</v>
+        <v>1.103578154425612</v>
       </c>
       <c r="J12" t="n">
-        <v>0.05178907721280603</v>
+        <v>1.103578154425612</v>
       </c>
       <c r="K12" t="n">
-        <v>0.05178907721280603</v>
+        <v>1.103578154425612</v>
       </c>
       <c r="L12" t="inlineStr"/>
     </row>

</xml_diff>